<commit_message>
Updated parts list and improved instructions
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/GitHub/poseidon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C20B3E-BF39-A34E-B315-6E33A06F3D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF66205-D6DD-FD4E-85DD-41293EB9B944}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53860" yWindow="7480" windowWidth="34120" windowHeight="18620" xr2:uid="{3282401A-40A0-594C-82D4-29FD74DF252F}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -798,11 +798,11 @@
         <v>3.99</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>3.99</v>
+        <v>7.98</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -1084,7 +1084,7 @@
     <row r="26" spans="1:5">
       <c r="C26" s="2">
         <f>SUM(C2:C25)</f>
-        <v>379.53999999999996</v>
+        <v>383.53</v>
       </c>
     </row>
     <row r="28" spans="1:5">

</xml_diff>